<commit_message>
Test mit gcc, Anpassungen
</commit_message>
<xml_diff>
--- a/Docs/Auswertung.xlsx
+++ b/Docs/Auswertung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\GitHub\Vergleichsprogramm\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274CE9F6-58BA-4738-98A9-8B8C3622E5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144668A1-0CE1-42CC-8EC4-C9D943F66B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="11333" activeTab="1" xr2:uid="{388948E0-F48B-4D39-A8BF-521842870DDC}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11332" activeTab="1" xr2:uid="{388948E0-F48B-4D39-A8BF-521842870DDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Ergebnisse für Lesetest" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Write</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Modern C++</t>
-  </si>
-  <si>
-    <t>0.541604</t>
   </si>
 </sst>
 </file>
@@ -760,7 +757,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -821,7 +818,7 @@
         <v>2.1536219999999999</v>
       </c>
       <c r="I2" s="12">
-        <v>7.6536999999999994E-2</v>
+        <v>7.3742000000000002E-2</v>
       </c>
       <c r="J2" s="4">
         <v>0.98143400000000003</v>
@@ -831,11 +828,11 @@
       </c>
       <c r="M2" s="17">
         <f>ROUND(K2/I2,1)</f>
-        <v>12.7</v>
+        <v>13.2</v>
       </c>
       <c r="O2" s="2">
         <f>C2-I2</f>
-        <v>2.6250000000000009E-2</v>
+        <v>2.9045000000000001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
@@ -932,7 +929,7 @@
         <v>12.17784</v>
       </c>
       <c r="I5" s="12">
-        <v>0.42164499999999999</v>
+        <v>0.362848</v>
       </c>
       <c r="J5" s="4">
         <v>1.985722</v>
@@ -942,11 +939,11 @@
       </c>
       <c r="M5" s="17">
         <f>ROUND(K5/I5,1)</f>
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" si="0"/>
-        <v>-0.20350699999999999</v>
+        <v>-0.14471000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
@@ -968,8 +965,8 @@
       <c r="G6" s="12">
         <v>1.297598</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>26</v>
+      <c r="I6" s="12">
+        <v>0.22040299999999999</v>
       </c>
       <c r="J6" s="4">
         <v>1.3489249999999999</v>
@@ -1000,7 +997,7 @@
         <v>20.076326000000002</v>
       </c>
       <c r="I7" s="12">
-        <v>0.72522900000000001</v>
+        <v>0.75720100000000001</v>
       </c>
       <c r="J7" s="5">
         <v>7.962974</v>
@@ -1010,11 +1007,11 @@
       </c>
       <c r="M7" s="17">
         <f>ROUND(K7/I7,1)</f>
-        <v>101.9</v>
+        <v>97.6</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" si="0"/>
-        <v>0.40759199999999984</v>
+        <v>0.37561999999999984</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.45">
@@ -1101,7 +1098,7 @@
         <v>4.9655999999999999E-2</v>
       </c>
       <c r="I10" s="12">
-        <v>9.2599999999999996E-4</v>
+        <v>8.9400000000000005E-4</v>
       </c>
       <c r="J10" s="4">
         <v>3.9500000000000004E-3</v>
@@ -1111,11 +1108,11 @@
       </c>
       <c r="M10" s="17">
         <f>ROUND(K10/I10,1)</f>
-        <v>4.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="O10" s="2">
         <f t="shared" si="0"/>
-        <v>7.2000000000000015E-5</v>
+        <v>1.0399999999999993E-4</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.45">
@@ -1138,7 +1135,7 @@
         <v>3.163E-3</v>
       </c>
       <c r="I11" s="12">
-        <v>1.34E-4</v>
+        <v>1.25E-4</v>
       </c>
       <c r="J11" s="4">
         <v>3.4699999999999998E-4</v>
@@ -1148,11 +1145,11 @@
       </c>
       <c r="M11" s="17">
         <f>ROUND(K11/I11,1)</f>
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="O11" s="2">
         <f t="shared" si="0"/>
-        <v>4.0999999999999994E-5</v>
+        <v>4.9999999999999996E-5</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.45">
@@ -1175,7 +1172,7 @@
         <v>6.3546999999999992E-2</v>
       </c>
       <c r="I12" s="12">
-        <v>2.1900000000000001E-3</v>
+        <v>1.877E-3</v>
       </c>
       <c r="J12" s="4">
         <v>5.293E-3</v>
@@ -1185,11 +1182,11 @@
       </c>
       <c r="M12" s="17">
         <f>ROUND(K12/I12,1)</f>
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="O12" s="2">
         <f t="shared" si="0"/>
-        <v>-6.4000000000000016E-4</v>
+        <v>-3.2700000000000003E-4</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.45">
@@ -1217,7 +1214,10 @@
         <f>SUM(G2:G12)</f>
         <v>44.010232999999999</v>
       </c>
-      <c r="I13" s="16"/>
+      <c r="I13" s="16">
+        <f>SUM(I2:I12)</f>
+        <v>1.641845</v>
+      </c>
       <c r="J13" s="4">
         <f>SUM(J2:J12)</f>
         <v>22.384626000000001</v>
@@ -1229,7 +1229,7 @@
       <c r="M13" s="17"/>
       <c r="O13" s="2">
         <f>SUM(O2:O12)</f>
-        <v>0.26553299999999991</v>
+        <v>0.2955069999999998</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
aktueller Stand Tests als Vektor mit Zeitangabe Parameter für Ausgabeverzeichnis
</commit_message>
<xml_diff>
--- a/Docs/Auswertung.xlsx
+++ b/Docs/Auswertung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\GitHub\Vergleichsprogramm\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144668A1-0CE1-42CC-8EC4-C9D943F66B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FD1947-8498-467F-9516-B3C9EF772A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11332" activeTab="1" xr2:uid="{388948E0-F48B-4D39-A8BF-521842870DDC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{388948E0-F48B-4D39-A8BF-521842870DDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Ergebnisse für Lesetest" sheetId="2" r:id="rId1"/>
@@ -757,7 +757,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1033,7 +1033,9 @@
       <c r="G8" s="12">
         <v>0.153339</v>
       </c>
-      <c r="I8" s="12"/>
+      <c r="I8" s="12">
+        <v>6.4102999999999993E-2</v>
+      </c>
       <c r="J8" s="4">
         <v>6.8253999999999995E-2</v>
       </c>
@@ -1065,7 +1067,9 @@
       <c r="G9" s="12">
         <v>5.6912979999999997</v>
       </c>
-      <c r="I9" s="12"/>
+      <c r="I9" s="12">
+        <v>0.197606</v>
+      </c>
       <c r="J9" s="4">
         <v>3.438993</v>
       </c>
@@ -1216,7 +1220,7 @@
       </c>
       <c r="I13" s="16">
         <f>SUM(I2:I12)</f>
-        <v>1.641845</v>
+        <v>1.903554</v>
       </c>
       <c r="J13" s="4">
         <f>SUM(J2:J12)</f>

</xml_diff>

<commit_message>
Korrektur, Ergänzungen 17.4. Verwendung von std::format Eingangsdaten überprüft (ranges) Ausgabe geprüft (begonnen) Fehlerkorrektur in ReadFromDirectory 2. Anwendung für vTune - Check
</commit_message>
<xml_diff>
--- a/Docs/Auswertung.xlsx
+++ b/Docs/Auswertung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\GitHub\Vergleichsprogramm\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD458B9-B1CE-46B2-A565-0077C9BDEB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32425DE9-C691-4971-9B2A-92768153BAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{388948E0-F48B-4D39-A8BF-521842870DDC}"/>
   </bookViews>
@@ -757,7 +757,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1041,7 +1041,7 @@
         <v>0.153339</v>
       </c>
       <c r="I8" s="4">
-        <v>2.2568000000000001E-2</v>
+        <v>2.0759E-2</v>
       </c>
       <c r="J8" s="4">
         <v>6.8253999999999995E-2</v>
@@ -1051,11 +1051,11 @@
       </c>
       <c r="M8" s="17">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="1"/>
-        <v>1.1399999999999987E-3</v>
+        <v>2.9490000000000002E-3</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
@@ -1081,7 +1081,7 @@
         <v>5.6912979999999997</v>
       </c>
       <c r="I9" s="4">
-        <v>0.18345800000000001</v>
+        <v>0.17763300000000001</v>
       </c>
       <c r="J9" s="4">
         <v>3.438993</v>
@@ -1091,11 +1091,11 @@
       </c>
       <c r="M9" s="17">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="O9" s="2">
         <f t="shared" si="1"/>
-        <v>-3.6126000000000019E-2</v>
+        <v>-3.0301000000000022E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="I13" s="16">
         <f>SUM(I2:I12)</f>
-        <v>1.4104479999999999</v>
+        <v>1.4028139999999998</v>
       </c>
       <c r="J13" s="4">
         <f>SUM(J2:J12)</f>
@@ -1251,11 +1251,11 @@
       </c>
       <c r="M13" s="17">
         <f t="shared" si="0"/>
-        <v>63.2</v>
+        <v>63.6</v>
       </c>
       <c r="O13" s="2">
         <f>SUM(O2:O12)</f>
-        <v>0.67697699999999994</v>
+        <v>0.68461099999999986</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">

</xml_diff>